<commit_message>
solved maven java v issue
</commit_message>
<xml_diff>
--- a/src/main/java/webAutomation/Elearning/unitbv/Utillities/SearchBook.xlsx
+++ b/src/main/java/webAutomation/Elearning/unitbv/Utillities/SearchBook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="12345"/>
+    <workbookView windowWidth="18960" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>user</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>55</t>
-  </si>
-  <si>
-    <t>Test from excel 2</t>
-  </si>
-  <si>
-    <t>20</t>
   </si>
 </sst>
 </file>
@@ -75,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -98,6 +92,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -105,7 +106,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,22 +122,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,6 +151,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -203,16 +204,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,7 +214,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -242,187 +236,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,17 +441,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,6 +484,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -519,17 +517,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,148 +532,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1012,13 +1006,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="42.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="24.8571428571429" customWidth="1"/>
@@ -1077,36 +1071,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="ionela.chiriac@student.unitbv.ro"/>
-    <hyperlink ref="A3" r:id="rId1" display="ionela.chiriac@student.unitbv.ro"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>